<commit_message>
Aggiornamento dati versione 2.1
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111XXXX646502CIAFFI_SRL/CIAFFI_SRL/LUITECOLAB/2.1/report-checklist.xlsx
+++ b/GATEWAY/A1#111XXXX646502CIAFFI_SRL/CIAFFI_SRL/LUITECOLAB/2.1/report-checklist.xlsx
@@ -278,13 +278,13 @@
 </t>
   </si>
   <si>
-    <t>2025-05-22T13:48:23Z</t>
-  </si>
-  <si>
-    <t>e9f7d206a5ae691b5c2fe0bc0b92a83c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.25413009308a4bae125585955d301f246db200fe149e896215630000f3b5c431.a5d629f814^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T16:42:22Z</t>
+  </si>
+  <si>
+    <t>a596c8f8ac81296b28a9651f8aee3e49</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.d805b83dc7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -504,13 +504,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-05-12T14:25:20Z</t>
-  </si>
-  <si>
-    <t>2abff759721e14cf4e6afd9cc3dc118b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.3606261b18^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T16:42:26Z</t>
+  </si>
+  <si>
+    <t>fab1d4d6df88ae72039454832fbd5605</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.b7bec97ac6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE ERRORE FORMALE CODICE FISCALE</t>
@@ -526,13 +526,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-05-09T09:06:24Z</t>
-  </si>
-  <si>
-    <t>ce2dbf04bf119209c0b89d9ccd9ec523</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.e2b26f8051^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T16:42:30Z</t>
+  </si>
+  <si>
+    <t>ef28cc5056285d668f0103299c9d3df7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.37de4f405c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE MANCA IL COMUNE DI RESIDENZA</t>
@@ -548,13 +548,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-05-09T09:08:02Z</t>
-  </si>
-  <si>
-    <t>24943690b6d99363d7e3193728e8a1df</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.cba3a4bc8f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T16:42:33Z</t>
+  </si>
+  <si>
+    <t>c90af6648d857871c6e036c535d6978b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.25384211b2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE MANCA IL NOME DEL PAZIENTE</t>
@@ -567,13 +567,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-05-09T09:09:16Z</t>
-  </si>
-  <si>
-    <t>ea789b4583569c72c376460af9afe2d3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.3dbdfcd50a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T16:42:37Z</t>
+  </si>
+  <si>
+    <t>6d97a94f7224235342bd51bad0046a19</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.bfe87b7959^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE MANCA IL SESSO DEL PAZIENTE</t>
@@ -586,13 +586,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-05-09T09:11:24Z</t>
-  </si>
-  <si>
-    <t>7c8ae8ab860b98e1f4eced9461d09c9e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.4043cf18cd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T16:42:40Z</t>
+  </si>
+  <si>
+    <t>50a164fe8e635146e825c163283314aa</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.579aff2f4c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE ERRORE SULL'IDENTIFICATIVO UNIVOCO DELLA PRESCRIZIONE</t>
@@ -608,13 +608,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-05-09T09:12:21Z</t>
-  </si>
-  <si>
-    <t>65b7f36a06fe71bca965d340b8157beb</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.b40e844989^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T16:42:43Z</t>
+  </si>
+  <si>
+    <t>09faf5d94a22415ec8221b313f2c781e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.3c50c80f8e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE SPECIFICA ESAME NON CORRETTA</t>
@@ -630,13 +630,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-05-09T09:13:18Z</t>
-  </si>
-  <si>
-    <t>7fbf9aa54e7714342294e1aa644ebb0f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.f68c9c6a69^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T16:42:46Z</t>
+  </si>
+  <si>
+    <t>1b204ad88ab9ba2f44c9601b7b9a8a94</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.3a04b6f6fb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE MANCA LA SPECIFICA DEL TIPO DI CAMPIONE</t>
@@ -649,13 +649,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-05-09T09:14:13Z</t>
-  </si>
-  <si>
-    <t>ed85c21baa7c707660546343eb9f3cd5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.25413009308a4bae125585955d301f246db200fe149e896215630000f3b5c431.683ad8df8c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T16:42:52Z</t>
+  </si>
+  <si>
+    <t>7189bf29ef53793b63f344d2c5398a84</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.442c4bbd94^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE MANCA LA SPECIFICA DEL CODICE DELL'ESAME ISOLATO</t>
@@ -1562,13 +1562,13 @@
 </t>
   </si>
   <si>
-    <t>2025-05-21T17:23:16Z</t>
-  </si>
-  <si>
-    <t>b0b335b83a2bd62cf5740145123d9525</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.12dbe02e35^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T16:42:56Z</t>
+  </si>
+  <si>
+    <t>a798e4de4aace3983cd0d9eab053a516</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.13a42706bf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_VPS_CT30</t>
@@ -1711,13 +1711,13 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto nella sezione "CASO DI TEST 19" riportata nei documenti "casi di test LAB" e "CDA2_Referto Medicina di Laboratorio_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2025-06-06T11:00:21Z</t>
-  </si>
-  <si>
-    <t>2727cc18a4583582b4f33d16ca7133f1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.aa8bec23d0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2025-06-17T16:42:59Z</t>
+  </si>
+  <si>
+    <t>cb85f8d0ddbfacd2fab1ef4fe0ccaf80</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.36b752291d7ee2dc9561b9ac59cd51f261a178cbc78d7ab2c2415ef6cdeef302.8c8a600e49^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>ATTENZIONE CODICE DI PRIORITA' DELLA RICHIESTA ERRATO</t>
@@ -1850,11 +1850,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="d/m/yyyy"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -1934,16 +1934,31 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1957,31 +1972,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1995,54 +1988,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2057,7 +2004,51 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2071,8 +2062,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2127,13 +2127,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2151,7 +2163,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2163,7 +2187,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2175,19 +2199,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2199,13 +2211,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2223,13 +2229,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2241,25 +2247,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2271,13 +2277,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2295,19 +2301,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2631,6 +2631,39 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2661,25 +2694,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -2688,19 +2708,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2719,161 +2728,152 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="32" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4511,11 +4511,11 @@
   <dimension ref="A1:W752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4:D4"/>
+      <selection pane="bottomRight" activeCell="I190" sqref="I190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4533333333333" defaultRowHeight="15" customHeight="1"/>
@@ -4816,7 +4816,7 @@
         <v>49</v>
       </c>
       <c r="F10" s="33">
-        <v>45799</v>
+        <v>45825</v>
       </c>
       <c r="G10" s="33" t="s">
         <v>50</v>
@@ -5463,7 +5463,7 @@
         <v>84</v>
       </c>
       <c r="F27" s="34">
-        <v>45786</v>
+        <v>45825</v>
       </c>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
@@ -5793,7 +5793,7 @@
         <v>95</v>
       </c>
       <c r="F35" s="34">
-        <v>45789</v>
+        <v>45825</v>
       </c>
       <c r="G35" s="34" t="s">
         <v>96</v>
@@ -5854,7 +5854,7 @@
         <v>102</v>
       </c>
       <c r="F36" s="34">
-        <v>45786</v>
+        <v>45825</v>
       </c>
       <c r="G36" s="34" t="s">
         <v>103</v>
@@ -5915,7 +5915,7 @@
         <v>109</v>
       </c>
       <c r="F37" s="34">
-        <v>45786</v>
+        <v>45825</v>
       </c>
       <c r="G37" s="34" t="s">
         <v>110</v>
@@ -5976,7 +5976,7 @@
         <v>115</v>
       </c>
       <c r="F38" s="34">
-        <v>45786</v>
+        <v>45825</v>
       </c>
       <c r="G38" s="34" t="s">
         <v>116</v>
@@ -6037,7 +6037,7 @@
         <v>121</v>
       </c>
       <c r="F39" s="34">
-        <v>45786</v>
+        <v>45825</v>
       </c>
       <c r="G39" s="34" t="s">
         <v>122</v>
@@ -6098,7 +6098,7 @@
         <v>128</v>
       </c>
       <c r="F40" s="34">
-        <v>45786</v>
+        <v>45825</v>
       </c>
       <c r="G40" s="34" t="s">
         <v>129</v>
@@ -6159,7 +6159,7 @@
         <v>135</v>
       </c>
       <c r="F41" s="34">
-        <v>45786</v>
+        <v>45825</v>
       </c>
       <c r="G41" s="34" t="s">
         <v>136</v>
@@ -6220,7 +6220,7 @@
         <v>141</v>
       </c>
       <c r="F42" s="34">
-        <v>45786</v>
+        <v>45825</v>
       </c>
       <c r="G42" s="34" t="s">
         <v>142</v>
@@ -10988,7 +10988,7 @@
         <v>401</v>
       </c>
       <c r="F170" s="34">
-        <v>45798</v>
+        <v>45825</v>
       </c>
       <c r="G170" s="34" t="s">
         <v>402</v>
@@ -11742,7 +11742,7 @@
         <v>444</v>
       </c>
       <c r="F190" s="34">
-        <v>45814</v>
+        <v>45825</v>
       </c>
       <c r="G190" s="34" t="s">
         <v>445</v>

</xml_diff>